<commit_message>
Subindo mais exercicios de DATA (exercicios finais)
</commit_message>
<xml_diff>
--- a/Excel/DATA/Exercicios_DATA.xlsx
+++ b/Excel/DATA/Exercicios_DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\Downloads\Analista de Dados\Excel\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56C0F045-6FE3-4EC5-9B00-DDA48FFFD90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D9053D-DA1A-4834-9E38-1B4518AFED1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{BB5801B7-556A-4A04-9314-0569BD75015C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Data de emissão</t>
   </si>
@@ -66,6 +66,41 @@
   </si>
   <si>
     <t>Qual a data prevista para o dinheiro voltar para a conta?</t>
+  </si>
+  <si>
+    <t>Pgto boleto</t>
+  </si>
+  <si>
+    <t>Emissão do boleto</t>
+  </si>
+  <si>
+    <t>Data de Vencimento</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Quantos </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dias corridos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para efetuar o pagamento?</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -89,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +140,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,16 +177,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB4BC38-42E3-4687-87A4-355A541A2483}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,16 +538,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>45604</v>
       </c>
     </row>
@@ -510,7 +555,7 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>45625</v>
       </c>
     </row>
@@ -518,7 +563,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>45598</v>
       </c>
     </row>
@@ -541,7 +586,7 @@
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>45597</v>
       </c>
     </row>
@@ -557,7 +602,7 @@
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>45598</v>
       </c>
     </row>
@@ -565,15 +610,47 @@
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <f>WORKDAY(B10,B11,B12)</f>
         <v>45604</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="6">
+        <v>45512</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="6">
+        <v>45524</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <f>DAYS360(B18,B19)</f>
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>